<commit_message>
Adding Bond 1991 to the es calc scheme
</commit_message>
<xml_diff>
--- a/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
+++ b/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\Group-based-interventions\ES calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\301744\Descriptive coding schemes\Mikkel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="126">
   <si>
     <t>authors</t>
   </si>
@@ -327,53 +327,122 @@
     <t>The Manchester Short Assessment of Quality of Life</t>
   </si>
   <si>
-    <t>Emp/posttest</t>
-  </si>
-  <si>
-    <t>Emp/followup</t>
-  </si>
-  <si>
-    <t>Hop/posttest</t>
-  </si>
-  <si>
-    <t>Hop/followup</t>
-  </si>
-  <si>
-    <t>Lon/posttest</t>
-  </si>
-  <si>
-    <t>Lon/followup</t>
-  </si>
-  <si>
-    <t>Qua/posttest</t>
-  </si>
-  <si>
-    <t>Qua/followup</t>
-  </si>
-  <si>
-    <t>Sel/posttest</t>
-  </si>
-  <si>
-    <t>Sel/followup</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Gestel-Timmermans</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
     <t>Raw means</t>
+  </si>
+  <si>
+    <t>Emp/3 months</t>
+  </si>
+  <si>
+    <t>Hop/3 months</t>
+  </si>
+  <si>
+    <t>Emp/6 months</t>
+  </si>
+  <si>
+    <t>Hop/6 months</t>
+  </si>
+  <si>
+    <t>Lon/3 months</t>
+  </si>
+  <si>
+    <t>Lon/6 months</t>
+  </si>
+  <si>
+    <t>Qual/3 months</t>
+  </si>
+  <si>
+    <t>Qual/6 months</t>
+  </si>
+  <si>
+    <t>Self/3 months</t>
+  </si>
+  <si>
+    <t>Self/6 months</t>
+  </si>
+  <si>
+    <t>Bond et al.</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Hospital-setting (i.e out-patient)</t>
+  </si>
+  <si>
+    <t>31.5</t>
+  </si>
+  <si>
+    <t>Pre-diagnosed</t>
+  </si>
+  <si>
+    <t>Pricipally heterogeneous</t>
+  </si>
+  <si>
+    <t>QES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convenient </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>assertive community treatment (ACT)</t>
+  </si>
+  <si>
+    <t>reference groups (RG)</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>Single-therapist</t>
+  </si>
+  <si>
+    <t>Hospital days</t>
+  </si>
+  <si>
+    <t>Hospital data</t>
+  </si>
+  <si>
+    <t>Paired t-tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-treatment number of hospital days </t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>ROBINS-I</t>
+  </si>
+  <si>
+    <t>Bond 1991</t>
+  </si>
+  <si>
+    <t>Gestel-Timmermans 2012</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Moderate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +482,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -456,23 +531,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,10 +835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ11"/>
+  <dimension ref="A1:AZ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO3" sqref="AO3:AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,12 +852,12 @@
     <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
@@ -786,13 +868,13 @@
     <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.85546875" style="1" customWidth="1"/>
     <col min="26" max="26" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" style="1" customWidth="1"/>
     <col min="32" max="32" width="8.7109375" style="1" customWidth="1"/>
     <col min="33" max="33" width="15.42578125" style="1" customWidth="1"/>
     <col min="34" max="34" width="11.85546875" style="1" customWidth="1"/>
@@ -801,11 +883,11 @@
     <col min="37" max="37" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.85546875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="37.7109375" style="1" customWidth="1"/>
     <col min="42" max="42" width="14.7109375" style="1" customWidth="1"/>
     <col min="43" max="43" width="11.85546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="20" style="1" customWidth="1"/>
+    <col min="44" max="44" width="28.42578125" style="1" customWidth="1"/>
     <col min="45" max="51" width="13.140625" style="1" customWidth="1"/>
     <col min="52" max="52" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="53" max="16384" width="9.140625" style="1"/>
@@ -941,8 +1023,8 @@
       <c r="AQ1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AR1" s="6" t="s">
-        <v>99</v>
+      <c r="AR1" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="AS1" s="2" t="s">
         <v>42</v>
@@ -969,7 +1051,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -1018,116 +1100,116 @@
       <c r="P2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="U2" s="6">
+        <v>1</v>
+      </c>
+      <c r="V2" s="6">
+        <v>1</v>
+      </c>
+      <c r="W2" s="6">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z2" s="6">
         <v>7</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AA2" s="6">
         <v>12</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="6">
         <v>2</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AC2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AF2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AI2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AK2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AL2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AM2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AN2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AN2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AR2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AU2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AV2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AX2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AY2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -1176,116 +1258,116 @@
       <c r="P3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="1" t="s">
+      <c r="U3" s="6">
+        <v>1</v>
+      </c>
+      <c r="V3" s="6">
+        <v>1</v>
+      </c>
+      <c r="W3" s="6">
+        <v>1</v>
+      </c>
+      <c r="X3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="Z3" s="6">
         <v>7</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="6">
         <v>12</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="6">
         <v>2</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AC3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AE3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AF3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AM3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AW3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AX3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1334,116 +1416,116 @@
       <c r="P4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U4" s="1">
-        <v>1</v>
-      </c>
-      <c r="V4" s="1">
-        <v>1</v>
-      </c>
-      <c r="W4" s="1">
-        <v>1</v>
-      </c>
-      <c r="X4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="1" t="s">
+      <c r="U4" s="6">
+        <v>1</v>
+      </c>
+      <c r="V4" s="6">
+        <v>1</v>
+      </c>
+      <c r="W4" s="6">
+        <v>1</v>
+      </c>
+      <c r="X4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="Z4" s="6">
         <v>7</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="6">
         <v>12</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="6">
         <v>2</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AC4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AE4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AF4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AH4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AI4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AJ4" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AK4" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AL4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AM4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AN4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AN4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AO4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AR4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AT4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AU4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AV4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX4" s="1" t="s">
+      <c r="AX4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY4" s="1" t="s">
+      <c r="AY4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ4" s="1" t="s">
+      <c r="AZ4" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>55</v>
       </c>
@@ -1492,116 +1574,116 @@
       <c r="P5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U5" s="1">
-        <v>1</v>
-      </c>
-      <c r="V5" s="1">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="1" t="s">
+      <c r="U5" s="6">
+        <v>1</v>
+      </c>
+      <c r="V5" s="6">
+        <v>1</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="Z5" s="6">
         <v>7</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AA5" s="6">
         <v>12</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="6">
         <v>2</v>
       </c>
-      <c r="AC5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AC5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AE5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AF5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AH5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AI5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AK5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AL5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AM5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AR5" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AT5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AU5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW5" s="1" t="s">
+      <c r="AV5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX5" s="1" t="s">
+      <c r="AX5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY5" s="1" t="s">
+      <c r="AY5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ5" s="1" t="s">
+      <c r="AZ5" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
@@ -1650,116 +1732,116 @@
       <c r="P6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U6" s="1">
-        <v>1</v>
-      </c>
-      <c r="V6" s="1">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1">
-        <v>1</v>
-      </c>
-      <c r="X6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="1" t="s">
+      <c r="U6" s="6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="Z6" s="6">
         <v>7</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="6">
         <v>12</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="6">
         <v>2</v>
       </c>
-      <c r="AC6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AC6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AE6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AF6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AH6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AI6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="AK6" s="1" t="s">
+      <c r="AK6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AL6" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AM6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AN6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
+      <c r="AN6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS6" s="1" t="s">
+      <c r="AR6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT6" s="1" t="s">
+      <c r="AT6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AU6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW6" s="1" t="s">
+      <c r="AV6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" s="1" t="s">
+      <c r="AX6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY6" s="1" t="s">
+      <c r="AY6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="1" t="s">
+      <c r="AZ6" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1808,116 +1890,116 @@
       <c r="P7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U7" s="1">
-        <v>1</v>
-      </c>
-      <c r="V7" s="1">
-        <v>1</v>
-      </c>
-      <c r="W7" s="1">
-        <v>1</v>
-      </c>
-      <c r="X7" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="1" t="s">
+      <c r="U7" s="6">
+        <v>1</v>
+      </c>
+      <c r="V7" s="6">
+        <v>1</v>
+      </c>
+      <c r="W7" s="6">
+        <v>1</v>
+      </c>
+      <c r="X7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="Z7" s="6">
         <v>7</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AA7" s="6">
         <v>12</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="6">
         <v>2</v>
       </c>
-      <c r="AC7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AC7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AE7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AF7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AH7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AI7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ7" s="3" t="s">
+      <c r="AJ7" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AK7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AL7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="AM7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AR7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT7" s="1" t="s">
+      <c r="AT7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU7" s="1" t="s">
+      <c r="AU7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW7" s="1" t="s">
+      <c r="AV7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="AX7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY7" s="1" t="s">
+      <c r="AY7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ7" s="1" t="s">
+      <c r="AZ7" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
@@ -1966,116 +2048,116 @@
       <c r="P8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U8" s="1">
-        <v>1</v>
-      </c>
-      <c r="V8" s="1">
-        <v>1</v>
-      </c>
-      <c r="W8" s="1">
-        <v>1</v>
-      </c>
-      <c r="X8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="1" t="s">
+      <c r="U8" s="6">
+        <v>1</v>
+      </c>
+      <c r="V8" s="6">
+        <v>1</v>
+      </c>
+      <c r="W8" s="6">
+        <v>1</v>
+      </c>
+      <c r="X8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="Z8" s="6">
         <v>7</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AA8" s="6">
         <v>12</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="6">
         <v>2</v>
       </c>
-      <c r="AC8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AC8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AF8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AH8" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AI8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AJ8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AK8" s="1" t="s">
+      <c r="AK8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AL8" s="1" t="s">
+      <c r="AL8" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AM8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AN8" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ8" s="1" t="s">
+      <c r="AN8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS8" s="1" t="s">
+      <c r="AR8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT8" s="1" t="s">
+      <c r="AT8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU8" s="1" t="s">
+      <c r="AU8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW8" s="1" t="s">
+      <c r="AV8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX8" s="1" t="s">
+      <c r="AX8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY8" s="1" t="s">
+      <c r="AY8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ8" s="1" t="s">
+      <c r="AZ8" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
@@ -2124,116 +2206,116 @@
       <c r="P9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U9" s="1">
-        <v>1</v>
-      </c>
-      <c r="V9" s="1">
-        <v>1</v>
-      </c>
-      <c r="W9" s="1">
-        <v>1</v>
-      </c>
-      <c r="X9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="1" t="s">
+      <c r="U9" s="6">
+        <v>1</v>
+      </c>
+      <c r="V9" s="6">
+        <v>1</v>
+      </c>
+      <c r="W9" s="6">
+        <v>1</v>
+      </c>
+      <c r="X9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="Z9" s="6">
         <v>7</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AA9" s="6">
         <v>12</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9" s="6">
         <v>2</v>
       </c>
-      <c r="AC9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AC9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AE9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AF9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="1" t="s">
+      <c r="AH9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI9" s="1" t="s">
+      <c r="AI9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ9" s="1" t="s">
+      <c r="AJ9" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AK9" s="1" t="s">
+      <c r="AK9" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AL9" s="1" t="s">
+      <c r="AL9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
+      <c r="AM9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS9" s="1" t="s">
+      <c r="AR9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT9" s="1" t="s">
+      <c r="AT9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU9" s="1" t="s">
+      <c r="AU9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW9" s="1" t="s">
+      <c r="AV9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX9" s="1" t="s">
+      <c r="AX9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY9" s="1" t="s">
+      <c r="AY9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ9" s="1" t="s">
+      <c r="AZ9" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -2282,116 +2364,116 @@
       <c r="P10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U10" s="1">
-        <v>1</v>
-      </c>
-      <c r="V10" s="1">
-        <v>1</v>
-      </c>
-      <c r="W10" s="1">
-        <v>1</v>
-      </c>
-      <c r="X10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="1" t="s">
+      <c r="U10" s="6">
+        <v>1</v>
+      </c>
+      <c r="V10" s="6">
+        <v>1</v>
+      </c>
+      <c r="W10" s="6">
+        <v>1</v>
+      </c>
+      <c r="X10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="Z10" s="6">
         <v>7</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AA10" s="6">
         <v>12</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AB10" s="6">
         <v>2</v>
       </c>
-      <c r="AC10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AC10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE10" s="1" t="s">
+      <c r="AE10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF10" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AF10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AH10" s="1" t="s">
+      <c r="AH10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI10" s="1" t="s">
+      <c r="AI10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ10" s="1" t="s">
+      <c r="AJ10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AK10" s="1" t="s">
+      <c r="AK10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AL10" s="1" t="s">
+      <c r="AL10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM10" s="1" t="s">
+      <c r="AM10" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AN10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
+      <c r="AN10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AQ10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AR10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS10" s="1" t="s">
+      <c r="AR10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AT10" s="1" t="s">
+      <c r="AT10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AU10" s="1" t="s">
+      <c r="AU10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AV10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW10" s="1" t="s">
+      <c r="AV10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AX10" s="1" t="s">
+      <c r="AX10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY10" s="1" t="s">
+      <c r="AY10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ10" s="1" t="s">
+      <c r="AZ10" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>55</v>
       </c>
@@ -2440,113 +2522,429 @@
       <c r="P11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U11" s="1">
-        <v>1</v>
-      </c>
-      <c r="V11" s="1">
-        <v>1</v>
-      </c>
-      <c r="W11" s="1">
-        <v>1</v>
-      </c>
-      <c r="X11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="1" t="s">
+      <c r="U11" s="6">
+        <v>1</v>
+      </c>
+      <c r="V11" s="6">
+        <v>1</v>
+      </c>
+      <c r="W11" s="6">
+        <v>1</v>
+      </c>
+      <c r="X11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="Z11" s="6">
         <v>7</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AA11" s="6">
         <v>12</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AB11" s="6">
         <v>2</v>
       </c>
-      <c r="AC11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AC11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AE11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AF11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AF11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AH11" s="1" t="s">
+      <c r="AH11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI11" s="1" t="s">
+      <c r="AI11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ11" s="1" t="s">
+      <c r="AJ11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AK11" s="1" t="s">
+      <c r="AK11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AL11" s="1" t="s">
+      <c r="AL11" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AM11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN11" s="1" t="s">
+      <c r="AM11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ11" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AO11" s="1" t="s">
+      <c r="B12" s="4">
+        <v>1991</v>
+      </c>
+      <c r="C12" s="4">
+        <v>73497493</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" s="4">
+        <v>79</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U12" s="4">
+        <v>1</v>
+      </c>
+      <c r="V12" s="4">
+        <v>1</v>
+      </c>
+      <c r="W12" s="4">
+        <v>2</v>
+      </c>
+      <c r="X12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>6</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AP11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AZ11" s="1" t="s">
-        <v>52</v>
+      <c r="AN12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AS12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AT12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV12" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AX12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ12" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1991</v>
+      </c>
+      <c r="C13" s="4">
+        <v>73497493</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K13" s="4">
+        <v>79</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U13" s="4">
+        <v>1</v>
+      </c>
+      <c r="V13" s="4">
+        <v>1</v>
+      </c>
+      <c r="W13" s="4">
+        <v>2</v>
+      </c>
+      <c r="X13" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AS13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AT13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV13" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AX13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ13" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding first es calc for Bond
</commit_message>
<xml_diff>
--- a/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
+++ b/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
@@ -1070,7 +1070,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" style="25" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
@@ -6033,7 +6033,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="21">
-        <v>943494</v>
+        <v>73490732</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>55</v>
@@ -6221,7 +6221,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="21">
-        <v>943494</v>
+        <v>73490732</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>55</v>
@@ -6409,7 +6409,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="21">
-        <v>943494</v>
+        <v>73490732</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>55</v>
@@ -6597,7 +6597,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="21">
-        <v>943494</v>
+        <v>73490732</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Adding covariates for Bond 2015
</commit_message>
<xml_diff>
--- a/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
+++ b/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="224">
   <si>
     <t>authors</t>
   </si>
@@ -677,12 +677,63 @@
   <si>
     <t>Barbic et al. 2009</t>
   </si>
+  <si>
+    <t xml:space="preserve">Bond et al. </t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>42.96</t>
+  </si>
+  <si>
+    <t>44.66</t>
+  </si>
+  <si>
+    <t>Schizophrenia spectrum, bipolar or other psychotic disorder and either significant treatment history or significant functional impairments</t>
+  </si>
+  <si>
+    <t>referrel from psychiatric services</t>
+  </si>
+  <si>
+    <t>Work Choice</t>
+  </si>
+  <si>
+    <t>Not clearly specified</t>
+  </si>
+  <si>
+    <t>Individual Placement and Support (IPS)</t>
+  </si>
+  <si>
+    <t>Post-intervention</t>
+  </si>
+  <si>
+    <t>Psychiatric hospitalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment </t>
+  </si>
+  <si>
+    <t>Days hospitalized</t>
+  </si>
+  <si>
+    <t>Risk of Psychiatric Hospitalization</t>
+  </si>
+  <si>
+    <t>Raw events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post-intervention events </t>
+  </si>
+  <si>
+    <t>Bond et al. 2015</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +792,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -790,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -851,6 +913,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,9 +1145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1112,10 +1189,10 @@
     <col min="35" max="35" width="19.7109375" customWidth="1"/>
     <col min="36" max="36" width="15.5703125" customWidth="1"/>
     <col min="37" max="37" width="30.85546875" customWidth="1"/>
-    <col min="38" max="38" width="18" customWidth="1"/>
+    <col min="38" max="38" width="35" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="6.42578125" customWidth="1"/>
     <col min="40" max="40" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="22.5703125" customWidth="1"/>
+    <col min="41" max="41" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.7109375" customWidth="1"/>
     <col min="43" max="43" width="19" customWidth="1"/>
     <col min="44" max="44" width="58.7109375" customWidth="1"/>
@@ -1124,9 +1201,9 @@
     <col min="47" max="47" width="27.140625" customWidth="1"/>
     <col min="48" max="48" width="35.7109375" customWidth="1"/>
     <col min="49" max="49" width="8.7109375" customWidth="1"/>
-    <col min="50" max="50" width="16.7109375" customWidth="1"/>
+    <col min="50" max="50" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="59.5703125" customWidth="1"/>
-    <col min="52" max="52" width="23.140625" customWidth="1"/>
+    <col min="52" max="52" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="8.85546875" customWidth="1"/>
     <col min="54" max="54" width="27.85546875" customWidth="1"/>
     <col min="55" max="59" width="14" customWidth="1"/>
@@ -1455,8 +1532,8 @@
       <c r="AR2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AS2" s="8" t="s">
-        <v>79</v>
+      <c r="AS2" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT2" s="8" t="s">
         <v>80</v>
@@ -1831,8 +1908,8 @@
       <c r="AR4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AS4" s="8" t="s">
-        <v>79</v>
+      <c r="AS4" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT4" s="8" t="s">
         <v>80</v>
@@ -2207,8 +2284,8 @@
       <c r="AR6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AS6" s="8" t="s">
-        <v>79</v>
+      <c r="AS6" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT6" s="8" t="s">
         <v>80</v>
@@ -2583,8 +2660,8 @@
       <c r="AR8" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AS8" s="8" t="s">
-        <v>79</v>
+      <c r="AS8" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT8" s="8" t="s">
         <v>80</v>
@@ -2959,8 +3036,8 @@
       <c r="AR10" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AS10" s="8" t="s">
-        <v>79</v>
+      <c r="AS10" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT10" s="8" t="s">
         <v>80</v>
@@ -4839,8 +4916,8 @@
       <c r="AR20" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="AS20" s="8" t="s">
-        <v>79</v>
+      <c r="AS20" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT20" s="8" t="s">
         <v>80</v>
@@ -5027,8 +5104,8 @@
       <c r="AR21" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AS21" s="8" t="s">
-        <v>79</v>
+      <c r="AS21" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT21" s="8" t="s">
         <v>80</v>
@@ -5403,8 +5480,8 @@
       <c r="AR23" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="AS23" s="8" t="s">
-        <v>79</v>
+      <c r="AS23" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT23" s="8" t="s">
         <v>80</v>
@@ -5779,8 +5856,8 @@
       <c r="AR25" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="AS25" s="8" t="s">
-        <v>79</v>
+      <c r="AS25" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT25" s="8" t="s">
         <v>80</v>
@@ -6155,8 +6232,8 @@
       <c r="AR27" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="AS27" s="16" t="s">
-        <v>79</v>
+      <c r="AS27" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT27" s="12" t="s">
         <v>80</v>
@@ -6343,8 +6420,8 @@
       <c r="AR28" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="AS28" s="16" t="s">
-        <v>79</v>
+      <c r="AS28" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT28" s="12" t="s">
         <v>80</v>
@@ -6531,8 +6608,8 @@
       <c r="AR29" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="AS29" s="16" t="s">
-        <v>79</v>
+      <c r="AS29" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT29" s="12" t="s">
         <v>80</v>
@@ -6719,8 +6796,8 @@
       <c r="AR30" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="AS30" s="16" t="s">
-        <v>79</v>
+      <c r="AS30" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="AT30" s="12" t="s">
         <v>80</v>
@@ -6774,261 +6851,741 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="6"/>
-      <c r="AD31" s="6"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="6"/>
-      <c r="AG31" s="6"/>
-      <c r="AH31" s="6"/>
-      <c r="AI31" s="6"/>
-      <c r="AJ31" s="6"/>
-      <c r="AK31" s="6"/>
-      <c r="AL31" s="6"/>
-      <c r="AM31" s="8"/>
-      <c r="AN31" s="6"/>
-      <c r="AO31" s="6"/>
-      <c r="AP31" s="6"/>
-      <c r="AQ31" s="6"/>
-      <c r="AR31" s="6"/>
-      <c r="AS31" s="6"/>
-      <c r="AT31" s="6"/>
-      <c r="AU31" s="6"/>
-      <c r="AV31" s="6"/>
-      <c r="AW31" s="6"/>
-      <c r="AX31" s="6"/>
-      <c r="AY31" s="6"/>
-      <c r="AZ31" s="6"/>
-      <c r="BA31" s="6"/>
-      <c r="BB31" s="6"/>
-      <c r="BC31" s="6"/>
-      <c r="BD31" s="6"/>
-      <c r="BE31" s="6"/>
-      <c r="BF31" s="6"/>
-      <c r="BG31" s="6"/>
-      <c r="BH31" s="6"/>
-      <c r="BI31" s="6"/>
-      <c r="BJ31" s="6"/>
-    </row>
-    <row r="32" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32" s="6"/>
-      <c r="AG32" s="6"/>
-      <c r="AH32" s="6"/>
-      <c r="AI32" s="6"/>
-      <c r="AJ32" s="6"/>
-      <c r="AK32" s="6"/>
-      <c r="AL32" s="6"/>
-      <c r="AM32" s="8"/>
-      <c r="AN32" s="6"/>
-      <c r="AO32" s="6"/>
-      <c r="AP32" s="6"/>
-      <c r="AQ32" s="6"/>
-      <c r="AR32" s="6"/>
-      <c r="AS32" s="6"/>
-      <c r="AT32" s="6"/>
-      <c r="AU32" s="6"/>
-      <c r="AV32" s="6"/>
-      <c r="AW32" s="6"/>
-      <c r="AX32" s="6"/>
-      <c r="AY32" s="6"/>
-      <c r="AZ32" s="6"/>
-      <c r="BA32" s="6"/>
-      <c r="BB32" s="6"/>
-      <c r="BC32" s="6"/>
-      <c r="BD32" s="6"/>
-      <c r="BE32" s="6"/>
-      <c r="BF32" s="6"/>
-      <c r="BG32" s="6"/>
-      <c r="BH32" s="6"/>
-      <c r="BI32" s="6"/>
-      <c r="BJ32" s="6"/>
-    </row>
-    <row r="33" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
-      <c r="AF33" s="6"/>
-      <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-      <c r="AI33" s="6"/>
-      <c r="AJ33" s="6"/>
-      <c r="AK33" s="6"/>
-      <c r="AL33" s="6"/>
-      <c r="AM33" s="8"/>
-      <c r="AN33" s="6"/>
-      <c r="AO33" s="6"/>
-      <c r="AP33" s="6"/>
-      <c r="AQ33" s="6"/>
-      <c r="AR33" s="6"/>
-      <c r="AS33" s="6"/>
-      <c r="AT33" s="6"/>
-      <c r="AU33" s="6"/>
-      <c r="AV33" s="6"/>
-      <c r="AW33" s="6"/>
-      <c r="AX33" s="6"/>
-      <c r="AY33" s="6"/>
-      <c r="AZ33" s="6"/>
-      <c r="BA33" s="6"/>
-      <c r="BB33" s="6"/>
-      <c r="BC33" s="6"/>
-      <c r="BD33" s="6"/>
-      <c r="BE33" s="6"/>
-      <c r="BF33" s="6"/>
-      <c r="BG33" s="6"/>
-      <c r="BH33" s="6"/>
-      <c r="BI33" s="6"/>
-      <c r="BJ33" s="6"/>
-    </row>
-    <row r="34" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
-      <c r="AC34" s="6"/>
-      <c r="AD34" s="6"/>
-      <c r="AE34" s="6"/>
-      <c r="AF34" s="6"/>
-      <c r="AG34" s="6"/>
-      <c r="AH34" s="6"/>
-      <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
-      <c r="AL34" s="6"/>
-      <c r="AM34" s="8"/>
-      <c r="AN34" s="6"/>
-      <c r="AO34" s="6"/>
-      <c r="AP34" s="6"/>
-      <c r="AQ34" s="6"/>
-      <c r="AR34" s="6"/>
-      <c r="AS34" s="6"/>
-      <c r="AT34" s="6"/>
-      <c r="AU34" s="6"/>
-      <c r="AV34" s="6"/>
-      <c r="AW34" s="6"/>
-      <c r="AX34" s="6"/>
-      <c r="AY34" s="6"/>
-      <c r="AZ34" s="6"/>
-      <c r="BA34" s="6"/>
-      <c r="BB34" s="6"/>
-      <c r="BC34" s="6"/>
-      <c r="BD34" s="6"/>
-      <c r="BE34" s="6"/>
-      <c r="BF34" s="6"/>
-      <c r="BG34" s="6"/>
-      <c r="BH34" s="6"/>
-      <c r="BI34" s="6"/>
-      <c r="BJ34" s="6"/>
+    <row r="31" spans="1:62" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="28">
+        <v>2015</v>
+      </c>
+      <c r="C31" s="29">
+        <v>5</v>
+      </c>
+      <c r="D31" s="26">
+        <v>73503724</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27">
+        <v>77</v>
+      </c>
+      <c r="Q31" s="27">
+        <v>82</v>
+      </c>
+      <c r="R31" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U31" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V31" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W31" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="X31" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y31" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z31" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF31" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG31" s="27">
+        <v>22</v>
+      </c>
+      <c r="AH31" s="27">
+        <v>52</v>
+      </c>
+      <c r="AI31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK31" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL31" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM31" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="AO31" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="AP31" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ31" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR31" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS31" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT31" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU31" s="27">
+        <v>12</v>
+      </c>
+      <c r="AV31" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX31" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY31" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ31" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="BA31" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB31" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC31" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD31" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE31" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF31" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG31" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH31" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI31" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ31" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:62" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="28">
+        <v>2015</v>
+      </c>
+      <c r="C32" s="29">
+        <v>5</v>
+      </c>
+      <c r="D32" s="26">
+        <v>73503724</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="N32" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27">
+        <v>77</v>
+      </c>
+      <c r="Q32" s="27">
+        <v>82</v>
+      </c>
+      <c r="R32" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="S32" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U32" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V32" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W32" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="X32" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y32" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z32" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE32" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF32" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG32" s="27">
+        <v>22</v>
+      </c>
+      <c r="AH32" s="27">
+        <v>52</v>
+      </c>
+      <c r="AI32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK32" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL32" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM32" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="AO32" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="AP32" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ32" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="AR32" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AS32" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT32" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU32" s="27">
+        <v>12</v>
+      </c>
+      <c r="AV32" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX32" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="AY32" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ32" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="BA32" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB32" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC32" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD32" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE32" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF32" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG32" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH32" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI32" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ32" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:62" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="28">
+        <v>2015</v>
+      </c>
+      <c r="C33" s="29">
+        <v>5</v>
+      </c>
+      <c r="D33" s="26">
+        <v>73503724</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27">
+        <v>77</v>
+      </c>
+      <c r="Q33" s="27">
+        <v>82</v>
+      </c>
+      <c r="R33" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="S33" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U33" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V33" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="X33" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y33" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z33" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF33" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG33" s="27">
+        <v>22</v>
+      </c>
+      <c r="AH33" s="27">
+        <v>52</v>
+      </c>
+      <c r="AI33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK33" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL33" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM33" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="AO33" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="AP33" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ33" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="AR33" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AS33" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT33" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU33" s="27">
+        <v>12</v>
+      </c>
+      <c r="AV33" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX33" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="AY33" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ33" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="BA33" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB33" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC33" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD33" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE33" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF33" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG33" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH33" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI33" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ33" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:62" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="28">
+        <v>2015</v>
+      </c>
+      <c r="C34" s="29">
+        <v>5</v>
+      </c>
+      <c r="D34" s="26">
+        <v>73503724</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="N34" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27">
+        <v>77</v>
+      </c>
+      <c r="Q34" s="27">
+        <v>82</v>
+      </c>
+      <c r="R34" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="S34" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T34" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U34" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V34" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="X34" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y34" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z34" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF34" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG34" s="27">
+        <v>22</v>
+      </c>
+      <c r="AH34" s="27">
+        <v>52</v>
+      </c>
+      <c r="AI34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK34" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL34" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM34" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="AO34" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP34" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ34" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="AR34" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AS34" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT34" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU34" s="27">
+        <v>12</v>
+      </c>
+      <c r="AV34" s="27">
+        <v>0</v>
+      </c>
+      <c r="AW34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX34" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="AY34" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ34" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="BA34" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB34" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC34" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD34" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE34" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF34" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG34" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH34" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI34" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ34" s="26" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="35" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>

</xml_diff>

<commit_message>
Adding covariates to Craigie 2009
</commit_message>
<xml_diff>
--- a/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
+++ b/ES calc/Descriptive coding scheme for group-based interventions (data).xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="252">
   <si>
     <t>authors</t>
   </si>
@@ -728,12 +728,96 @@
   <si>
     <t>Bond et al. 2015</t>
   </si>
+  <si>
+    <t>Craigie &amp; Nathan</t>
+  </si>
+  <si>
+    <t>Public funded</t>
+  </si>
+  <si>
+    <t>36.4</t>
+  </si>
+  <si>
+    <t>37.6</t>
+  </si>
+  <si>
+    <t>35.2</t>
+  </si>
+  <si>
+    <t>38.3</t>
+  </si>
+  <si>
+    <t>Major depressive disorder, anixiety, social phobia, OCD, PTSD, panic disorder, dysthymia</t>
+  </si>
+  <si>
+    <t>QES</t>
+  </si>
+  <si>
+    <t>were referred according to the normal day-to-day clinic referral process (p. 304)</t>
+  </si>
+  <si>
+    <t>Group CBT</t>
+  </si>
+  <si>
+    <t>Cognitive-behavior therapy</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinical professionals </t>
+  </si>
+  <si>
+    <t>Individual CBT</t>
+  </si>
+  <si>
+    <t>Beck Depression Inventory-II (BDI-II)</t>
+  </si>
+  <si>
+    <t>Beck Anxiety Inventory (BAI)</t>
+  </si>
+  <si>
+    <t>Quality of Life Enjoyment and Satisfaction Questionnaire (Q-LES-Q)</t>
+  </si>
+  <si>
+    <t>Quality of Life</t>
+  </si>
+  <si>
+    <t>ITT/BDI-II</t>
+  </si>
+  <si>
+    <t>ITT/BAI</t>
+  </si>
+  <si>
+    <t>ITT/QoL</t>
+  </si>
+  <si>
+    <t>TOT/BDI-II</t>
+  </si>
+  <si>
+    <t>TOT/BAI</t>
+  </si>
+  <si>
+    <t>TOT/QoL</t>
+  </si>
+  <si>
+    <t>ROBINS-I</t>
+  </si>
+  <si>
+    <t>Craigie &amp; Nathan 2009</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,6 +887,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -852,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,6 +1019,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,9 +1237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AY1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB38" sqref="BB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1252,7 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -1169,13 +1261,13 @@
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="117.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.7109375" customWidth="1"/>
     <col min="20" max="20" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="35.42578125" customWidth="1"/>
     <col min="22" max="22" width="7.140625" customWidth="1"/>
     <col min="23" max="23" width="14.140625" customWidth="1"/>
-    <col min="24" max="24" width="31.28515625" customWidth="1"/>
+    <col min="24" max="24" width="77.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.7109375" customWidth="1"/>
     <col min="26" max="26" width="17.28515625" customWidth="1"/>
     <col min="27" max="27" width="11.28515625" customWidth="1"/>
@@ -1204,10 +1296,10 @@
     <col min="50" max="50" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="59.5703125" customWidth="1"/>
     <col min="52" max="52" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.85546875" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="27.85546875" customWidth="1"/>
     <col min="55" max="59" width="14" customWidth="1"/>
-    <col min="60" max="61" width="3.7109375" customWidth="1"/>
+    <col min="60" max="61" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1399,7 +1491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -1587,7 +1679,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>54</v>
       </c>
@@ -1775,7 +1867,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -1963,7 +2055,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>54</v>
       </c>
@@ -2151,7 +2243,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -2339,7 +2431,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2527,7 +2619,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
@@ -2715,7 +2807,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -2903,7 +2995,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -3091,7 +3183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
@@ -3279,7 +3371,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>110</v>
       </c>
@@ -3467,7 +3559,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>131</v>
       </c>
@@ -3655,7 +3747,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>131</v>
       </c>
@@ -3843,7 +3935,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>110</v>
       </c>
@@ -4031,7 +4123,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>131</v>
       </c>
@@ -4219,7 +4311,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>110</v>
       </c>
@@ -4407,7 +4499,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>110</v>
       </c>
@@ -4595,7 +4687,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>110</v>
       </c>
@@ -4783,7 +4875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>110</v>
       </c>
@@ -4971,7 +5063,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>153</v>
       </c>
@@ -5159,7 +5251,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>153</v>
       </c>
@@ -5347,7 +5439,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>153</v>
       </c>
@@ -5535,7 +5627,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>153</v>
       </c>
@@ -5723,7 +5815,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>153</v>
       </c>
@@ -5911,7 +6003,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>153</v>
       </c>
@@ -6099,7 +6191,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>181</v>
       </c>
@@ -6287,7 +6379,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>181</v>
       </c>
@@ -6475,7 +6567,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>181</v>
       </c>
@@ -6663,7 +6755,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:62" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>181</v>
       </c>
@@ -6851,7 +6943,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:62" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:62" s="26" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>207</v>
       </c>
@@ -6885,14 +6977,18 @@
       <c r="K31" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="L31" s="27"/>
+      <c r="L31" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="M31" s="27" t="s">
         <v>209</v>
       </c>
       <c r="N31" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="O31" s="27"/>
+      <c r="O31" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="P31" s="27">
         <v>77</v>
       </c>
@@ -7035,7 +7131,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:62" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:62" s="32" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>207</v>
       </c>
@@ -7069,14 +7165,18 @@
       <c r="K32" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="L32" s="27"/>
+      <c r="L32" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="M32" s="27" t="s">
         <v>209</v>
       </c>
       <c r="N32" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="O32" s="27"/>
+      <c r="O32" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="P32" s="27">
         <v>77</v>
       </c>
@@ -7219,7 +7319,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:62" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:62" s="32" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>207</v>
       </c>
@@ -7253,14 +7353,18 @@
       <c r="K33" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="27"/>
+      <c r="L33" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="M33" s="27" t="s">
         <v>209</v>
       </c>
       <c r="N33" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="O33" s="27"/>
+      <c r="O33" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="P33" s="27">
         <v>77</v>
       </c>
@@ -7437,14 +7541,18 @@
       <c r="K34" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="27"/>
+      <c r="L34" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="M34" s="27" t="s">
         <v>209</v>
       </c>
       <c r="N34" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="O34" s="27"/>
+      <c r="O34" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="P34" s="27">
         <v>77</v>
       </c>
@@ -7587,389 +7695,1133 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6"/>
-      <c r="U35" s="6"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-      <c r="AA35" s="6"/>
-      <c r="AB35" s="6"/>
-      <c r="AC35" s="6"/>
-      <c r="AD35" s="6"/>
-      <c r="AE35" s="6"/>
-      <c r="AF35" s="6"/>
-      <c r="AG35" s="6"/>
-      <c r="AH35" s="6"/>
-      <c r="AI35" s="6"/>
-      <c r="AJ35" s="6"/>
-      <c r="AK35" s="6"/>
-      <c r="AL35" s="6"/>
-      <c r="AM35" s="8"/>
-      <c r="AN35" s="6"/>
-      <c r="AO35" s="6"/>
-      <c r="AP35" s="6"/>
-      <c r="AQ35" s="6"/>
-      <c r="AR35" s="6"/>
-      <c r="AS35" s="6"/>
-      <c r="AT35" s="6"/>
-      <c r="AU35" s="6"/>
-      <c r="AV35" s="6"/>
-      <c r="AW35" s="6"/>
-      <c r="AX35" s="6"/>
-      <c r="AY35" s="6"/>
-      <c r="AZ35" s="6"/>
-      <c r="BA35" s="6"/>
-      <c r="BB35" s="6"/>
-      <c r="BC35" s="6"/>
-      <c r="BD35" s="6"/>
-      <c r="BE35" s="6"/>
-      <c r="BF35" s="6"/>
-      <c r="BG35" s="6"/>
-      <c r="BH35" s="6"/>
-      <c r="BI35" s="6"/>
-      <c r="BJ35" s="6"/>
-    </row>
-    <row r="36" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AJ36" s="6"/>
-      <c r="AK36" s="6"/>
-      <c r="AL36" s="6"/>
-      <c r="AM36" s="8"/>
-      <c r="AN36" s="6"/>
-      <c r="AO36" s="6"/>
-      <c r="AP36" s="6"/>
-      <c r="AQ36" s="6"/>
-      <c r="AR36" s="6"/>
-      <c r="AS36" s="6"/>
-      <c r="AT36" s="6"/>
-      <c r="AU36" s="6"/>
-      <c r="AV36" s="6"/>
-      <c r="AW36" s="6"/>
-      <c r="AX36" s="6"/>
-      <c r="AY36" s="6"/>
-      <c r="AZ36" s="6"/>
-      <c r="BA36" s="6"/>
-      <c r="BB36" s="6"/>
-      <c r="BC36" s="6"/>
-      <c r="BD36" s="6"/>
-      <c r="BE36" s="6"/>
-      <c r="BF36" s="6"/>
-      <c r="BG36" s="6"/>
-      <c r="BH36" s="6"/>
-      <c r="BI36" s="6"/>
-      <c r="BJ36" s="6"/>
-    </row>
-    <row r="37" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-      <c r="AA37" s="6"/>
-      <c r="AB37" s="6"/>
-      <c r="AC37" s="6"/>
-      <c r="AD37" s="6"/>
-      <c r="AE37" s="6"/>
-      <c r="AF37" s="6"/>
-      <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
-      <c r="AI37" s="6"/>
-      <c r="AJ37" s="6"/>
-      <c r="AK37" s="6"/>
-      <c r="AL37" s="6"/>
-      <c r="AM37" s="8"/>
-      <c r="AN37" s="6"/>
-      <c r="AO37" s="6"/>
-      <c r="AP37" s="6"/>
-      <c r="AQ37" s="6"/>
-      <c r="AR37" s="6"/>
-      <c r="AS37" s="6"/>
-      <c r="AT37" s="6"/>
-      <c r="AU37" s="6"/>
-      <c r="AV37" s="6"/>
-      <c r="AW37" s="6"/>
-      <c r="AX37" s="6"/>
-      <c r="AY37" s="6"/>
-      <c r="AZ37" s="6"/>
-      <c r="BA37" s="6"/>
-      <c r="BB37" s="6"/>
-      <c r="BC37" s="6"/>
-      <c r="BD37" s="6"/>
-      <c r="BE37" s="6"/>
-      <c r="BF37" s="6"/>
-      <c r="BG37" s="6"/>
-      <c r="BH37" s="6"/>
-      <c r="BI37" s="6"/>
-      <c r="BJ37" s="6"/>
-    </row>
-    <row r="38" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
-      <c r="AB38" s="6"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="6"/>
-      <c r="AE38" s="6"/>
-      <c r="AF38" s="6"/>
-      <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
-      <c r="AI38" s="6"/>
-      <c r="AJ38" s="6"/>
-      <c r="AK38" s="6"/>
-      <c r="AL38" s="6"/>
-      <c r="AM38" s="8"/>
-      <c r="AN38" s="6"/>
-      <c r="AO38" s="6"/>
-      <c r="AP38" s="6"/>
-      <c r="AQ38" s="6"/>
-      <c r="AR38" s="6"/>
-      <c r="AS38" s="6"/>
-      <c r="AT38" s="6"/>
-      <c r="AU38" s="6"/>
-      <c r="AV38" s="6"/>
-      <c r="AW38" s="6"/>
-      <c r="AX38" s="6"/>
-      <c r="AY38" s="6"/>
-      <c r="AZ38" s="6"/>
-      <c r="BA38" s="6"/>
-      <c r="BB38" s="6"/>
-      <c r="BC38" s="6"/>
-      <c r="BD38" s="6"/>
-      <c r="BE38" s="6"/>
-      <c r="BF38" s="6"/>
-      <c r="BG38" s="6"/>
-      <c r="BH38" s="6"/>
-      <c r="BI38" s="6"/>
-      <c r="BJ38" s="6"/>
-    </row>
-    <row r="39" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
-      <c r="AE39" s="6"/>
-      <c r="AF39" s="6"/>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-      <c r="AI39" s="6"/>
-      <c r="AJ39" s="6"/>
-      <c r="AK39" s="6"/>
-      <c r="AL39" s="6"/>
-      <c r="AM39" s="8"/>
-      <c r="AN39" s="6"/>
-      <c r="AO39" s="6"/>
-      <c r="AP39" s="6"/>
-      <c r="AQ39" s="6"/>
-      <c r="AR39" s="6"/>
-      <c r="AS39" s="6"/>
-      <c r="AT39" s="6"/>
-      <c r="AU39" s="6"/>
-      <c r="AV39" s="6"/>
-      <c r="AW39" s="6"/>
-      <c r="AX39" s="6"/>
-      <c r="AY39" s="6"/>
-      <c r="AZ39" s="6"/>
-      <c r="BA39" s="6"/>
-      <c r="BB39" s="6"/>
-      <c r="BC39" s="6"/>
-      <c r="BD39" s="6"/>
-      <c r="BE39" s="6"/>
-      <c r="BF39" s="6"/>
-      <c r="BG39" s="6"/>
-      <c r="BH39" s="6"/>
-      <c r="BI39" s="6"/>
-      <c r="BJ39" s="6"/>
-    </row>
-    <row r="40" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="6"/>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
-      <c r="AE40" s="6"/>
-      <c r="AF40" s="6"/>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-      <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
-      <c r="AK40" s="6"/>
-      <c r="AL40" s="6"/>
-      <c r="AM40" s="8"/>
-      <c r="AN40" s="6"/>
-      <c r="AO40" s="6"/>
-      <c r="AP40" s="6"/>
-      <c r="AQ40" s="6"/>
-      <c r="AR40" s="6"/>
-      <c r="AS40" s="6"/>
-      <c r="AT40" s="6"/>
-      <c r="AU40" s="6"/>
-      <c r="AV40" s="6"/>
-      <c r="AW40" s="6"/>
-      <c r="AX40" s="6"/>
-      <c r="AY40" s="6"/>
-      <c r="AZ40" s="6"/>
-      <c r="BA40" s="6"/>
-      <c r="BB40" s="6"/>
-      <c r="BC40" s="6"/>
-      <c r="BD40" s="6"/>
-      <c r="BE40" s="6"/>
-      <c r="BF40" s="6"/>
-      <c r="BG40" s="6"/>
-      <c r="BH40" s="6"/>
-      <c r="BI40" s="6"/>
-      <c r="BJ40" s="6"/>
+    <row r="35" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B35" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C35" s="18">
+        <v>7</v>
+      </c>
+      <c r="D35" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K35" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="M35" s="16">
+        <v>34</v>
+      </c>
+      <c r="N35" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="O35" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P35" s="16">
+        <v>40</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>33</v>
+      </c>
+      <c r="R35" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S35" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T35" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U35" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V35" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W35" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X35" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y35" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z35" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA35" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF35" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG35" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH35" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI35" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK35" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL35" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM35" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN35" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO35" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP35" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ35" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR35" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS35" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT35" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU35" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV35" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX35" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ35" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="BA35" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB35" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC35" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD35" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE35" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF35" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG35" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH35" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI35" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ35" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C36" s="18">
+        <v>7</v>
+      </c>
+      <c r="D36" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K36" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="M36" s="16">
+        <v>34</v>
+      </c>
+      <c r="N36" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="O36" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P36" s="16">
+        <v>40</v>
+      </c>
+      <c r="Q36" s="16">
+        <v>33</v>
+      </c>
+      <c r="R36" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S36" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T36" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U36" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V36" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W36" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X36" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y36" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z36" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA36" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF36" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG36" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH36" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI36" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK36" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL36" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM36" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN36" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO36" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ36" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR36" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS36" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT36" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU36" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV36" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW36" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX36" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ36" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="BA36" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB36" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC36" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD36" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF36" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH36" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI36" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ36" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C37" s="18">
+        <v>7</v>
+      </c>
+      <c r="D37" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K37" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="M37" s="16">
+        <v>34</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="O37" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P37" s="16">
+        <v>40</v>
+      </c>
+      <c r="Q37" s="16">
+        <v>33</v>
+      </c>
+      <c r="R37" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S37" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U37" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V37" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W37" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X37" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y37" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z37" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA37" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF37" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG37" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH37" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI37" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK37" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL37" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM37" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN37" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO37" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AP37" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ37" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR37" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="AS37" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT37" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU37" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV37" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW37" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX37" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ37" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="BA37" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB37" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC37" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD37" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE37" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF37" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG37" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH37" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI37" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ37" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C38" s="18">
+        <v>7</v>
+      </c>
+      <c r="D38" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="O38" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P38" s="16">
+        <v>38</v>
+      </c>
+      <c r="Q38" s="16">
+        <v>32</v>
+      </c>
+      <c r="R38" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S38" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U38" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V38" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W38" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X38" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y38" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z38" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE38" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF38" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG38" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH38" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK38" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL38" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM38" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO38" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP38" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ38" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR38" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS38" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT38" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU38" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV38" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW38" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX38" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY38" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ38" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="BA38" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB38" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC38" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD38" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE38" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF38" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG38" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH38" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI38" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ38" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C39" s="18">
+        <v>7</v>
+      </c>
+      <c r="D39" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K39" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="O39" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P39" s="16">
+        <v>38</v>
+      </c>
+      <c r="Q39" s="16">
+        <v>32</v>
+      </c>
+      <c r="R39" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S39" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U39" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V39" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W39" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X39" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y39" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z39" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE39" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF39" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG39" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH39" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK39" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL39" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM39" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN39" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO39" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP39" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ39" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR39" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS39" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT39" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU39" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV39" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW39" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX39" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ39" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="BA39" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB39" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC39" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD39" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE39" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF39" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG39" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH39" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI39" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ39" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:62" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="20">
+        <v>2009</v>
+      </c>
+      <c r="C40" s="18">
+        <v>7</v>
+      </c>
+      <c r="D40" s="21">
+        <v>73502127</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="O40" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P40" s="16">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="16">
+        <v>32</v>
+      </c>
+      <c r="R40" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S40" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T40" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="U40" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="V40" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="W40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="X40" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z40" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF40" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG40" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH40" s="16">
+        <v>10</v>
+      </c>
+      <c r="AI40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK40" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL40" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM40" s="18">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO40" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AP40" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ40" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR40" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="AS40" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AT40" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU40" s="16">
+        <v>14</v>
+      </c>
+      <c r="AV40" s="16">
+        <v>4</v>
+      </c>
+      <c r="AW40" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX40" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ40" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA40" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BB40" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="BC40" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="BD40" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE40" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF40" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG40" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH40" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI40" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ40" s="16" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="41" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>

</xml_diff>